<commit_message>
ordered logistic analysis of the transmission of ILK
</commit_message>
<xml_diff>
--- a/processedData/data.xlsx
+++ b/processedData/data.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\R\Informing-the-use-of-ILK-in-Ecosystems-Sustainability-in-West-Africa\processedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08AB7B5-F2D8-4EEE-ADDF-19D694937737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A78B5-D0BD-41AB-806E-0625E972B793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{E6975BF4-9BEB-4FA3-8222-9153DCF5476F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6975BF4-9BEB-4FA3-8222-9153DCF5476F}"/>
   </bookViews>
   <sheets>
     <sheet name="dataprocessed" sheetId="1" r:id="rId1"/>
-    <sheet name="SEC" sheetId="2" r:id="rId2"/>
-    <sheet name="statusILK" sheetId="3" r:id="rId3"/>
-    <sheet name="fieldsILK" sheetId="4" r:id="rId4"/>
+    <sheet name="transmissionILK" sheetId="5" r:id="rId2"/>
+    <sheet name="mainActors" sheetId="6" r:id="rId3"/>
+    <sheet name="SEC" sheetId="2" r:id="rId4"/>
+    <sheet name="statusILK" sheetId="3" r:id="rId5"/>
+    <sheet name="fieldsILK" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataprocessed!$A$1:$EI$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">transmissionILK!$A$1:$L$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3229" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="513">
   <si>
     <t>First Name</t>
   </si>
@@ -1583,6 +1586,12 @@
   </si>
   <si>
     <t>placeSeedOperate</t>
+  </si>
+  <si>
+    <t>Craftmen</t>
+  </si>
+  <si>
+    <t>Teacher</t>
   </si>
 </sst>
 </file>
@@ -1940,8 +1949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC44064-31E2-4DA5-997E-F2038EC0F7F1}">
   <dimension ref="A1:EI71"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="CC53" workbookViewId="0">
+      <selection activeCell="BW1" sqref="BW1:CD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27903,6 +27912,4108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B523599-1209-4F95-9E66-35B7E6614C60}">
+  <dimension ref="A1:L71"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" t="s">
+        <v>411</v>
+      </c>
+      <c r="I1" t="s">
+        <v>458</v>
+      </c>
+      <c r="J1" t="s">
+        <v>437</v>
+      </c>
+      <c r="K1" t="s">
+        <v>438</v>
+      </c>
+      <c r="L1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>393</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>393</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>393</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>393</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>393</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>393</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>393</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>393</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>511</v>
+      </c>
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>49</v>
+      </c>
+      <c r="C16">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>393</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>95</v>
+      </c>
+      <c r="C17">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>393</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I17" t="s">
+        <v>137</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>66</v>
+      </c>
+      <c r="C18">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>393</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>393</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>393</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>393</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>95</v>
+      </c>
+      <c r="C23">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>393</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>393</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>393</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>71</v>
+      </c>
+      <c r="C26">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>393</v>
+      </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>71</v>
+      </c>
+      <c r="C27">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>394</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>189</v>
+      </c>
+      <c r="H28" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>393</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>393</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>393</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31">
+        <v>5</v>
+      </c>
+      <c r="K31">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>394</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33">
+        <v>65</v>
+      </c>
+      <c r="C33">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>393</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33">
+        <v>5</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34">
+        <v>85</v>
+      </c>
+      <c r="C34">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
+        <v>393</v>
+      </c>
+      <c r="E34" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>55</v>
+      </c>
+      <c r="C35">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>393</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>393</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>393</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" t="s">
+        <v>66</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>393</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>393</v>
+      </c>
+      <c r="E39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" t="s">
+        <v>40</v>
+      </c>
+      <c r="I39" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>67</v>
+      </c>
+      <c r="C40">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>393</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>130</v>
+      </c>
+      <c r="H40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" t="s">
+        <v>31</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41">
+        <v>59</v>
+      </c>
+      <c r="C41">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
+        <v>393</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" t="s">
+        <v>137</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>393</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" t="s">
+        <v>130</v>
+      </c>
+      <c r="H42" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43">
+        <v>65</v>
+      </c>
+      <c r="C43">
+        <v>65</v>
+      </c>
+      <c r="D43" t="s">
+        <v>393</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>5</v>
+      </c>
+      <c r="L43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>393</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="K44">
+        <v>5</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>53</v>
+      </c>
+      <c r="C45">
+        <v>53</v>
+      </c>
+      <c r="D45" t="s">
+        <v>393</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>130</v>
+      </c>
+      <c r="H45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J45">
+        <v>5</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>393</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46" t="s">
+        <v>40</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="K46">
+        <v>5</v>
+      </c>
+      <c r="L46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>59</v>
+      </c>
+      <c r="C47">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>393</v>
+      </c>
+      <c r="E47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47">
+        <v>5</v>
+      </c>
+      <c r="K47">
+        <v>5</v>
+      </c>
+      <c r="L47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>49</v>
+      </c>
+      <c r="C48">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>393</v>
+      </c>
+      <c r="E48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" t="s">
+        <v>40</v>
+      </c>
+      <c r="I48" t="s">
+        <v>40</v>
+      </c>
+      <c r="J48">
+        <v>5</v>
+      </c>
+      <c r="K48">
+        <v>5</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>65</v>
+      </c>
+      <c r="C49">
+        <v>65</v>
+      </c>
+      <c r="D49" t="s">
+        <v>393</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" t="s">
+        <v>85</v>
+      </c>
+      <c r="H49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
+        <v>393</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>26</v>
+      </c>
+      <c r="C51">
+        <v>312</v>
+      </c>
+      <c r="D51" t="s">
+        <v>393</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" t="s">
+        <v>40</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <v>44</v>
+      </c>
+      <c r="D52" t="s">
+        <v>393</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" t="s">
+        <v>40</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+      <c r="K52">
+        <v>5</v>
+      </c>
+      <c r="L52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>68</v>
+      </c>
+      <c r="C53">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>393</v>
+      </c>
+      <c r="E53" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" t="s">
+        <v>40</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>49</v>
+      </c>
+      <c r="D54" t="s">
+        <v>393</v>
+      </c>
+      <c r="E54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" t="s">
+        <v>66</v>
+      </c>
+      <c r="I54" t="s">
+        <v>31</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>4</v>
+      </c>
+      <c r="L54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>40</v>
+      </c>
+      <c r="C55">
+        <v>40</v>
+      </c>
+      <c r="D55" t="s">
+        <v>394</v>
+      </c>
+      <c r="E55" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" t="s">
+        <v>130</v>
+      </c>
+      <c r="H55" t="s">
+        <v>40</v>
+      </c>
+      <c r="I55" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55">
+        <v>5</v>
+      </c>
+      <c r="K55">
+        <v>5</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>60</v>
+      </c>
+      <c r="D56" t="s">
+        <v>394</v>
+      </c>
+      <c r="E56" t="s">
+        <v>136</v>
+      </c>
+      <c r="F56" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57">
+        <v>64</v>
+      </c>
+      <c r="C57">
+        <v>64</v>
+      </c>
+      <c r="D57" t="s">
+        <v>394</v>
+      </c>
+      <c r="E57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" t="s">
+        <v>512</v>
+      </c>
+      <c r="H57" t="s">
+        <v>40</v>
+      </c>
+      <c r="I57" t="s">
+        <v>101</v>
+      </c>
+      <c r="J57">
+        <v>5</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>60</v>
+      </c>
+      <c r="D58" t="s">
+        <v>393</v>
+      </c>
+      <c r="E58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" t="s">
+        <v>130</v>
+      </c>
+      <c r="H58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>393</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" t="s">
+        <v>66</v>
+      </c>
+      <c r="I59" t="s">
+        <v>40</v>
+      </c>
+      <c r="J59">
+        <v>5</v>
+      </c>
+      <c r="K59">
+        <v>5</v>
+      </c>
+      <c r="L59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>50</v>
+      </c>
+      <c r="C60">
+        <v>50</v>
+      </c>
+      <c r="D60" t="s">
+        <v>393</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" t="s">
+        <v>66</v>
+      </c>
+      <c r="I60" t="s">
+        <v>40</v>
+      </c>
+      <c r="J60">
+        <v>5</v>
+      </c>
+      <c r="K60">
+        <v>4</v>
+      </c>
+      <c r="L60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61">
+        <v>48</v>
+      </c>
+      <c r="C61">
+        <v>48</v>
+      </c>
+      <c r="D61" t="s">
+        <v>393</v>
+      </c>
+      <c r="E61" t="s">
+        <v>136</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62">
+        <v>45</v>
+      </c>
+      <c r="C62">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>393</v>
+      </c>
+      <c r="E62" t="s">
+        <v>136</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" t="s">
+        <v>130</v>
+      </c>
+      <c r="H62" t="s">
+        <v>66</v>
+      </c>
+      <c r="I62" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+      <c r="K62">
+        <v>4</v>
+      </c>
+      <c r="L62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63">
+        <v>31</v>
+      </c>
+      <c r="C63">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>393</v>
+      </c>
+      <c r="E63" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63" t="s">
+        <v>66</v>
+      </c>
+      <c r="I63" t="s">
+        <v>101</v>
+      </c>
+      <c r="J63">
+        <v>5</v>
+      </c>
+      <c r="K63">
+        <v>5</v>
+      </c>
+      <c r="L63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64">
+        <v>50</v>
+      </c>
+      <c r="C64">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>393</v>
+      </c>
+      <c r="E64" t="s">
+        <v>136</v>
+      </c>
+      <c r="F64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" t="s">
+        <v>130</v>
+      </c>
+      <c r="H64" t="s">
+        <v>40</v>
+      </c>
+      <c r="I64" t="s">
+        <v>66</v>
+      </c>
+      <c r="J64">
+        <v>5</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65">
+        <v>74</v>
+      </c>
+      <c r="C65">
+        <v>74</v>
+      </c>
+      <c r="D65" t="s">
+        <v>393</v>
+      </c>
+      <c r="E65" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" t="s">
+        <v>130</v>
+      </c>
+      <c r="H65" t="s">
+        <v>40</v>
+      </c>
+      <c r="I65" t="s">
+        <v>40</v>
+      </c>
+      <c r="J65">
+        <v>5</v>
+      </c>
+      <c r="K65">
+        <v>5</v>
+      </c>
+      <c r="L65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66">
+        <v>77</v>
+      </c>
+      <c r="C66">
+        <v>77</v>
+      </c>
+      <c r="D66" t="s">
+        <v>393</v>
+      </c>
+      <c r="E66" t="s">
+        <v>136</v>
+      </c>
+      <c r="F66" t="s">
+        <v>100</v>
+      </c>
+      <c r="G66" t="s">
+        <v>130</v>
+      </c>
+      <c r="H66" t="s">
+        <v>66</v>
+      </c>
+      <c r="I66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66">
+        <v>5</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67">
+        <v>65</v>
+      </c>
+      <c r="C67">
+        <v>65</v>
+      </c>
+      <c r="D67" t="s">
+        <v>393</v>
+      </c>
+      <c r="E67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F67" t="s">
+        <v>100</v>
+      </c>
+      <c r="G67" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" t="s">
+        <v>66</v>
+      </c>
+      <c r="I67" t="s">
+        <v>66</v>
+      </c>
+      <c r="J67">
+        <v>5</v>
+      </c>
+      <c r="K67">
+        <v>5</v>
+      </c>
+      <c r="L67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68">
+        <v>40</v>
+      </c>
+      <c r="C68">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>393</v>
+      </c>
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" t="s">
+        <v>130</v>
+      </c>
+      <c r="H68" t="s">
+        <v>101</v>
+      </c>
+      <c r="I68" t="s">
+        <v>40</v>
+      </c>
+      <c r="J68">
+        <v>5</v>
+      </c>
+      <c r="K68">
+        <v>3</v>
+      </c>
+      <c r="L68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69">
+        <v>53</v>
+      </c>
+      <c r="C69">
+        <v>53</v>
+      </c>
+      <c r="D69" t="s">
+        <v>393</v>
+      </c>
+      <c r="E69" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" t="s">
+        <v>130</v>
+      </c>
+      <c r="H69" t="s">
+        <v>40</v>
+      </c>
+      <c r="I69" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69">
+        <v>5</v>
+      </c>
+      <c r="K69">
+        <v>4</v>
+      </c>
+      <c r="L69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70">
+        <v>80</v>
+      </c>
+      <c r="C70">
+        <v>80</v>
+      </c>
+      <c r="D70" t="s">
+        <v>393</v>
+      </c>
+      <c r="E70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
+        <v>100</v>
+      </c>
+      <c r="G70" t="s">
+        <v>130</v>
+      </c>
+      <c r="H70" t="s">
+        <v>40</v>
+      </c>
+      <c r="I70" t="s">
+        <v>40</v>
+      </c>
+      <c r="J70">
+        <v>5</v>
+      </c>
+      <c r="K70">
+        <v>2</v>
+      </c>
+      <c r="L70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71">
+        <v>62</v>
+      </c>
+      <c r="C71">
+        <v>24</v>
+      </c>
+      <c r="D71" t="s">
+        <v>393</v>
+      </c>
+      <c r="E71" t="s">
+        <v>27</v>
+      </c>
+      <c r="F71" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" t="s">
+        <v>130</v>
+      </c>
+      <c r="H71" t="s">
+        <v>31</v>
+      </c>
+      <c r="I71" t="s">
+        <v>40</v>
+      </c>
+      <c r="J71">
+        <v>5</v>
+      </c>
+      <c r="K71">
+        <v>4</v>
+      </c>
+      <c r="L71">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F80F95-B65F-42C6-A908-C73D9D09DDEA}">
+  <dimension ref="A1:H71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" t="s">
+        <v>465</v>
+      </c>
+      <c r="H1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>5</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>4</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>5</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>5</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>5</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>5</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <v>5</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <v>5</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <v>5</v>
+      </c>
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DD3BDC-24F7-4C43-BFCC-3B904B7FE560}">
   <dimension ref="A1:I71"/>
   <sheetViews>
@@ -29987,7 +34098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BE338F-D5B7-4474-ACAF-14DA79BA13DD}">
   <dimension ref="A1:K71"/>
   <sheetViews>
@@ -32149,12 +36260,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758660E5-8FD6-44FF-8CAE-13D5EA8EC242}">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection sqref="A1:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
main actors and threats scripts
</commit_message>
<xml_diff>
--- a/processedData/data.xlsx
+++ b/processedData/data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scripts\R\Informing-the-use-of-ILK-in-Ecosystems-Sustainability-in-West-Africa\processedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A78B5-D0BD-41AB-806E-0625E972B793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE18E3B5-C534-42DF-83A2-A669A9EC2867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{E6975BF4-9BEB-4FA3-8222-9153DCF5476F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{E6975BF4-9BEB-4FA3-8222-9153DCF5476F}"/>
   </bookViews>
   <sheets>
     <sheet name="dataprocessed" sheetId="1" r:id="rId1"/>
     <sheet name="transmissionILK" sheetId="5" r:id="rId2"/>
     <sheet name="mainActors" sheetId="6" r:id="rId3"/>
-    <sheet name="SEC" sheetId="2" r:id="rId4"/>
-    <sheet name="statusILK" sheetId="3" r:id="rId5"/>
-    <sheet name="fieldsILK" sheetId="4" r:id="rId6"/>
+    <sheet name="threats" sheetId="7" r:id="rId4"/>
+    <sheet name="SEC" sheetId="2" r:id="rId5"/>
+    <sheet name="statusILK" sheetId="3" r:id="rId6"/>
+    <sheet name="fieldsILK" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dataprocessed!$A$1:$EI$71</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3726" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3738" uniqueCount="513">
   <si>
     <t>First Name</t>
   </si>
@@ -1949,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC44064-31E2-4DA5-997E-F2038EC0F7F1}">
   <dimension ref="A1:EI71"/>
   <sheetViews>
-    <sheetView topLeftCell="CC53" workbookViewId="0">
-      <selection activeCell="BW1" sqref="BW1:CD71"/>
+    <sheetView topLeftCell="DN53" workbookViewId="0">
+      <selection activeCell="DF1" sqref="DF1:DQ71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30486,7 +30487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F80F95-B65F-42C6-A908-C73D9D09DDEA}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -32014,6 +32017,2237 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187A50E2-CE10-44FE-8BA1-CA2179F0E7BB}">
+  <dimension ref="A1:L71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D1" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1" t="s">
+        <v>495</v>
+      </c>
+      <c r="F1" t="s">
+        <v>496</v>
+      </c>
+      <c r="G1" t="s">
+        <v>497</v>
+      </c>
+      <c r="H1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I1" t="s">
+        <v>499</v>
+      </c>
+      <c r="J1" t="s">
+        <v>500</v>
+      </c>
+      <c r="K1" t="s">
+        <v>501</v>
+      </c>
+      <c r="L1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+      <c r="L41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="L46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <v>2</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>4</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <v>5</v>
+      </c>
+      <c r="L59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>3</v>
+      </c>
+      <c r="K60">
+        <v>5</v>
+      </c>
+      <c r="L60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>3</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>5</v>
+      </c>
+      <c r="L63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>2</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>2</v>
+      </c>
+      <c r="L64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+      <c r="K67">
+        <v>3</v>
+      </c>
+      <c r="L67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>4</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>5</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>5</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DD3BDC-24F7-4C43-BFCC-3B904B7FE560}">
   <dimension ref="A1:I71"/>
   <sheetViews>
@@ -34098,7 +36332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BE338F-D5B7-4474-ACAF-14DA79BA13DD}">
   <dimension ref="A1:K71"/>
   <sheetViews>
@@ -36260,7 +38494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758660E5-8FD6-44FF-8CAE-13D5EA8EC242}">
   <dimension ref="A1:L71"/>
   <sheetViews>

</xml_diff>